<commit_message>
Otras correcciones, pero estas son de las gráficas
</commit_message>
<xml_diff>
--- a/Resultados/resultados regresiones.xlsx
+++ b/Resultados/resultados regresiones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9f3ba38939858e1d/Desktop/Apps/R Studio/Analisis articulo/Resultados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1911" documentId="13_ncr:1_{92D13805-9BBE-4F41-8C85-8658F7E9C3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE36F905-66C4-4F80-B912-D659A842E7F6}"/>
+  <xr:revisionPtr revIDLastSave="1972" documentId="13_ncr:1_{92D13805-9BBE-4F41-8C85-8658F7E9C3DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88931E3B-9ADA-477D-80FB-98EAE8885F06}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="617" firstSheet="3" activeTab="9" xr2:uid="{B182AF77-74A8-47E2-B10D-FE90D360CEA8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="617" firstSheet="3" activeTab="8" xr2:uid="{B182AF77-74A8-47E2-B10D-FE90D360CEA8}"/>
   </bookViews>
   <sheets>
     <sheet name="SIMPLES" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1239" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="225">
   <si>
     <t>EDAD</t>
   </si>
@@ -971,7 +971,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1141,6 +1141,18 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1174,6 +1186,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1181,6 +1211,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1192,18 +1225,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1213,53 +1234,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1595,29 +1570,29 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70" t="s">
+      <c r="C1" s="74"/>
+      <c r="D1" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="70"/>
+      <c r="E1" s="74"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="70" t="s">
+      <c r="H1" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70" t="s">
+      <c r="I1" s="74"/>
+      <c r="J1" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="70"/>
-      <c r="M1" s="67" t="s">
+      <c r="K1" s="74"/>
+      <c r="M1" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="69"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="73"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -2016,10 +1991,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67D41627-2355-4EEA-A2CD-D2B21314CEDD}">
-  <dimension ref="A1:R129"/>
+  <dimension ref="A1:V129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O83" sqref="O83:R91"/>
+    <sheetView topLeftCell="F64" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V76" sqref="V76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2029,39 +2004,42 @@
     <col min="15" max="15" width="25" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="15" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.88671875" customWidth="1"/>
+    <col min="22" max="22" width="16.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="73"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="81" t="s">
+      <c r="C2" s="94"/>
+      <c r="D2" s="92" t="s">
         <v>121</v>
       </c>
-      <c r="E2" s="83"/>
-      <c r="F2" s="81" t="s">
+      <c r="E2" s="94"/>
+      <c r="F2" s="92" t="s">
         <v>118</v>
       </c>
-      <c r="G2" s="83"/>
-      <c r="H2" s="67" t="s">
+      <c r="G2" s="94"/>
+      <c r="H2" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="69"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="73"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -2435,36 +2413,36 @@
       <c r="G17" s="25"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="81" t="s">
+      <c r="A18" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="83"/>
+      <c r="B18" s="93"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="94"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="83"/>
-      <c r="D19" s="81" t="s">
+      <c r="C19" s="94"/>
+      <c r="D19" s="92" t="s">
         <v>121</v>
       </c>
-      <c r="E19" s="83"/>
-      <c r="F19" s="81" t="s">
+      <c r="E19" s="94"/>
+      <c r="F19" s="92" t="s">
         <v>118</v>
       </c>
-      <c r="G19" s="83"/>
-      <c r="H19" s="67" t="s">
+      <c r="G19" s="94"/>
+      <c r="H19" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="I19" s="68"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="69"/>
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="73"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
@@ -2811,36 +2789,36 @@
       <c r="K31" s="4"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="71" t="s">
+      <c r="A35" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="72"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="73"/>
+      <c r="B35" s="76"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="76"/>
+      <c r="F35" s="76"/>
+      <c r="G35" s="77"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" s="24"/>
-      <c r="B36" s="81" t="s">
+      <c r="B36" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="C36" s="83"/>
-      <c r="D36" s="81" t="s">
+      <c r="C36" s="94"/>
+      <c r="D36" s="92" t="s">
         <v>121</v>
       </c>
-      <c r="E36" s="83"/>
-      <c r="F36" s="81" t="s">
+      <c r="E36" s="94"/>
+      <c r="F36" s="92" t="s">
         <v>118</v>
       </c>
-      <c r="G36" s="83"/>
-      <c r="H36" s="67" t="s">
+      <c r="G36" s="94"/>
+      <c r="H36" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="I36" s="68"/>
-      <c r="J36" s="68"/>
-      <c r="K36" s="69"/>
+      <c r="I36" s="72"/>
+      <c r="J36" s="72"/>
+      <c r="K36" s="73"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
@@ -3218,36 +3196,36 @@
       <c r="G51" s="25"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" s="81" t="s">
+      <c r="A52" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="B52" s="82"/>
-      <c r="C52" s="82"/>
-      <c r="D52" s="82"/>
-      <c r="E52" s="82"/>
-      <c r="F52" s="82"/>
-      <c r="G52" s="83"/>
+      <c r="B52" s="93"/>
+      <c r="C52" s="93"/>
+      <c r="D52" s="93"/>
+      <c r="E52" s="93"/>
+      <c r="F52" s="93"/>
+      <c r="G52" s="94"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="24"/>
-      <c r="B53" s="81" t="s">
+      <c r="B53" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="C53" s="83"/>
-      <c r="D53" s="81" t="s">
+      <c r="C53" s="94"/>
+      <c r="D53" s="92" t="s">
         <v>121</v>
       </c>
-      <c r="E53" s="83"/>
-      <c r="F53" s="81" t="s">
+      <c r="E53" s="94"/>
+      <c r="F53" s="92" t="s">
         <v>118</v>
       </c>
-      <c r="G53" s="83"/>
-      <c r="H53" s="67" t="s">
+      <c r="G53" s="94"/>
+      <c r="H53" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="I53" s="68"/>
-      <c r="J53" s="68"/>
-      <c r="K53" s="69"/>
+      <c r="I53" s="72"/>
+      <c r="J53" s="72"/>
+      <c r="K53" s="73"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A54" s="24" t="s">
@@ -3562,7 +3540,7 @@
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65" s="46" t="s">
         <v>113</v>
       </c>
@@ -3589,74 +3567,88 @@
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
     </row>
-    <row r="69" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A69" s="87" t="s">
+    <row r="69" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="B69" s="88" t="s">
+      <c r="B69" s="95" t="s">
         <v>131</v>
       </c>
-      <c r="C69" s="89"/>
-      <c r="D69" s="89"/>
-      <c r="E69" s="89"/>
-      <c r="F69" s="89"/>
-      <c r="G69" s="90"/>
-      <c r="H69" s="88" t="s">
+      <c r="C69" s="96"/>
+      <c r="D69" s="96"/>
+      <c r="E69" s="96"/>
+      <c r="F69" s="96"/>
+      <c r="G69" s="97"/>
+      <c r="H69" s="95" t="s">
         <v>132</v>
       </c>
-      <c r="I69" s="89"/>
-      <c r="J69" s="89"/>
-      <c r="K69" s="89"/>
-      <c r="L69" s="89"/>
-      <c r="M69" s="90"/>
-      <c r="O69" s="87" t="s">
+      <c r="I69" s="96"/>
+      <c r="J69" s="96"/>
+      <c r="K69" s="96"/>
+      <c r="L69" s="96"/>
+      <c r="M69" s="97"/>
+      <c r="O69" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="P69" s="105" t="s">
+      <c r="P69" s="85" t="s">
         <v>139</v>
       </c>
-      <c r="Q69" s="106"/>
-      <c r="R69" s="107"/>
-    </row>
-    <row r="70" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A70" s="87"/>
-      <c r="B70" s="78" t="s">
+      <c r="Q69" s="86"/>
+      <c r="R69" s="87"/>
+      <c r="T69" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="C70" s="79"/>
-      <c r="D70" s="78" t="s">
+      <c r="U69" s="82" t="s">
+        <v>140</v>
+      </c>
+      <c r="V69" s="82"/>
+    </row>
+    <row r="70" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="82"/>
+      <c r="B70" s="88" t="s">
+        <v>116</v>
+      </c>
+      <c r="C70" s="89"/>
+      <c r="D70" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="E70" s="79"/>
-      <c r="F70" s="78" t="s">
+      <c r="E70" s="89"/>
+      <c r="F70" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="G70" s="79"/>
-      <c r="H70" s="78" t="s">
+      <c r="G70" s="89"/>
+      <c r="H70" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="I70" s="79"/>
-      <c r="J70" s="78" t="s">
+      <c r="I70" s="89"/>
+      <c r="J70" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="K70" s="79"/>
-      <c r="L70" s="78" t="s">
+      <c r="K70" s="89"/>
+      <c r="L70" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="M70" s="79"/>
-      <c r="O70" s="87"/>
+      <c r="M70" s="89"/>
+      <c r="O70" s="82"/>
       <c r="P70" s="49" t="s">
         <v>223</v>
       </c>
       <c r="Q70" s="49" t="s">
         <v>224</v>
       </c>
-      <c r="R70" s="84" t="s">
+      <c r="R70" s="83" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="71" spans="1:18" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A71" s="87"/>
+      <c r="T70" s="82"/>
+      <c r="U70" s="49" t="s">
+        <v>223</v>
+      </c>
+      <c r="V70" s="49" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A71" s="82"/>
       <c r="B71" s="49" t="s">
         <v>10</v>
       </c>
@@ -3693,16 +3685,23 @@
       <c r="M71" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="O71" s="87"/>
+      <c r="O71" s="82"/>
       <c r="P71" s="49" t="s">
         <v>137</v>
       </c>
       <c r="Q71" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="R71" s="86"/>
-    </row>
-    <row r="72" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="R71" s="84"/>
+      <c r="T71" s="82"/>
+      <c r="U71" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="V71" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="54" t="s">
         <v>127</v>
       </c>
@@ -3754,8 +3753,17 @@
       <c r="R72" s="63">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="73" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="T72" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="U72" s="65">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="V72" s="65">
+        <v>2.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="54" t="s">
         <v>104</v>
       </c>
@@ -3807,8 +3815,17 @@
       <c r="R73" s="63">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="74" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="T73" s="55" t="s">
+        <v>174</v>
+      </c>
+      <c r="U73" s="65">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="V73" s="65">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="54" t="s">
         <v>105</v>
       </c>
@@ -3848,14 +3865,14 @@
       <c r="M74" s="60">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="O74" s="104"/>
-      <c r="P74" s="105" t="s">
+      <c r="O74" s="70"/>
+      <c r="P74" s="85" t="s">
         <v>140</v>
       </c>
-      <c r="Q74" s="106"/>
-      <c r="R74" s="107"/>
-    </row>
-    <row r="75" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Q74" s="86"/>
+      <c r="R74" s="87"/>
+    </row>
+    <row r="75" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="54" t="s">
         <v>102</v>
       </c>
@@ -3908,7 +3925,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="76" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="54" t="s">
         <v>106</v>
       </c>
@@ -3961,7 +3978,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="77" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="54" t="s">
         <v>107</v>
       </c>
@@ -4014,7 +4031,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="78" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="54" t="s">
         <v>112</v>
       </c>
@@ -4067,7 +4084,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="79" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="54" t="s">
         <v>108</v>
       </c>
@@ -4108,7 +4125,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="54" t="s">
         <v>109</v>
       </c>
@@ -4149,7 +4166,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="81" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="54" t="s">
         <v>110</v>
       </c>
@@ -4193,7 +4210,7 @@
       <c r="Q81" s="64"/>
       <c r="R81" s="64"/>
     </row>
-    <row r="82" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="55" t="s">
         <v>113</v>
       </c>
@@ -4237,83 +4254,104 @@
       <c r="Q82" s="64"/>
       <c r="R82" s="64"/>
     </row>
-    <row r="83" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="O83" s="84" t="s">
+    <row r="83" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O83" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="P83" s="105" t="s">
+      <c r="P83" s="85" t="s">
         <v>170</v>
       </c>
-      <c r="Q83" s="106"/>
-      <c r="R83" s="107"/>
-    </row>
-    <row r="84" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="O84" s="85"/>
+      <c r="Q83" s="86"/>
+      <c r="R83" s="87"/>
+      <c r="T83" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="U83" s="82" t="s">
+        <v>170</v>
+      </c>
+      <c r="V83" s="82"/>
+    </row>
+    <row r="84" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O84" s="91"/>
       <c r="P84" s="49" t="s">
         <v>223</v>
       </c>
       <c r="Q84" s="49" t="s">
         <v>224</v>
       </c>
-      <c r="R84" s="84" t="s">
+      <c r="R84" s="83" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="85" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A85" s="87" t="s">
+      <c r="T84" s="82"/>
+      <c r="U84" s="49" t="s">
+        <v>223</v>
+      </c>
+      <c r="V84" s="49" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="85" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="B85" s="88" t="s">
+      <c r="B85" s="95" t="s">
         <v>131</v>
       </c>
-      <c r="C85" s="89"/>
-      <c r="D85" s="89"/>
-      <c r="E85" s="89"/>
-      <c r="F85" s="89"/>
-      <c r="G85" s="90"/>
-      <c r="H85" s="88" t="s">
+      <c r="C85" s="96"/>
+      <c r="D85" s="96"/>
+      <c r="E85" s="96"/>
+      <c r="F85" s="96"/>
+      <c r="G85" s="97"/>
+      <c r="H85" s="95" t="s">
         <v>132</v>
       </c>
-      <c r="I85" s="89"/>
-      <c r="J85" s="89"/>
-      <c r="K85" s="89"/>
-      <c r="L85" s="89"/>
-      <c r="M85" s="90"/>
-      <c r="O85" s="86"/>
+      <c r="I85" s="96"/>
+      <c r="J85" s="96"/>
+      <c r="K85" s="96"/>
+      <c r="L85" s="96"/>
+      <c r="M85" s="97"/>
+      <c r="O85" s="84"/>
       <c r="P85" s="49" t="s">
         <v>137</v>
       </c>
       <c r="Q85" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="R85" s="86"/>
-    </row>
-    <row r="86" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A86" s="87"/>
-      <c r="B86" s="78" t="s">
+      <c r="R85" s="84"/>
+      <c r="T85" s="82"/>
+      <c r="U85" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="V85" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="82"/>
+      <c r="B86" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="C86" s="79"/>
-      <c r="D86" s="78" t="s">
+      <c r="C86" s="89"/>
+      <c r="D86" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="E86" s="79"/>
-      <c r="F86" s="78" t="s">
+      <c r="E86" s="89"/>
+      <c r="F86" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="G86" s="79"/>
-      <c r="H86" s="78" t="s">
+      <c r="G86" s="89"/>
+      <c r="H86" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="I86" s="79"/>
-      <c r="J86" s="78" t="s">
+      <c r="I86" s="89"/>
+      <c r="J86" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="K86" s="79"/>
-      <c r="L86" s="78" t="s">
+      <c r="K86" s="89"/>
+      <c r="L86" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="M86" s="79"/>
+      <c r="M86" s="89"/>
       <c r="O86" s="54" t="s">
         <v>127</v>
       </c>
@@ -4326,9 +4364,18 @@
       <c r="R86" s="63">
         <v>2.0000000000000002E-5</v>
       </c>
-    </row>
-    <row r="87" spans="1:18" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A87" s="87"/>
+      <c r="T86" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="U86" s="98">
+        <v>0.09</v>
+      </c>
+      <c r="V86" s="98">
+        <v>3.0000000000000001E-6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:22" ht="18.600000000000001" x14ac:dyDescent="0.3">
+      <c r="A87" s="82"/>
       <c r="B87" s="49" t="s">
         <v>10</v>
       </c>
@@ -4377,8 +4424,13 @@
       <c r="R87" s="63">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="88" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="T87" s="70"/>
+      <c r="U87" s="82" t="s">
+        <v>171</v>
+      </c>
+      <c r="V87" s="82"/>
+    </row>
+    <row r="88" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="54" t="s">
         <v>127</v>
       </c>
@@ -4430,8 +4482,17 @@
       <c r="R88" s="63">
         <v>4.0000000000000001E-3</v>
       </c>
-    </row>
-    <row r="89" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="T88" s="54" t="s">
+        <v>154</v>
+      </c>
+      <c r="U88" s="65">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="V88" s="65">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="54" t="s">
         <v>104</v>
       </c>
@@ -4471,14 +4532,23 @@
       <c r="M89" s="48">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="O89" s="104"/>
-      <c r="P89" s="105" t="s">
+      <c r="O89" s="70"/>
+      <c r="P89" s="85" t="s">
         <v>171</v>
       </c>
-      <c r="Q89" s="106"/>
-      <c r="R89" s="107"/>
-    </row>
-    <row r="90" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Q89" s="86"/>
+      <c r="R89" s="87"/>
+      <c r="T89" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="U89" s="65">
+        <v>1E-4</v>
+      </c>
+      <c r="V89" s="65">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="54" t="s">
         <v>105</v>
       </c>
@@ -4531,7 +4601,7 @@
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="91" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="54" t="s">
         <v>102</v>
       </c>
@@ -4584,7 +4654,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="54" t="s">
         <v>106</v>
       </c>
@@ -4625,7 +4695,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="93" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="54" t="s">
         <v>107</v>
       </c>
@@ -4666,7 +4736,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="54" t="s">
         <v>112</v>
       </c>
@@ -4707,7 +4777,7 @@
         <v>8.9999999999999998E-4</v>
       </c>
     </row>
-    <row r="95" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="54" t="s">
         <v>108</v>
       </c>
@@ -4748,7 +4818,7 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="54" t="s">
         <v>109</v>
       </c>
@@ -4887,55 +4957,55 @@
       <c r="M99" s="57"/>
     </row>
     <row r="100" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A100" s="87" t="s">
+      <c r="A100" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="B100" s="78" t="s">
+      <c r="B100" s="88" t="s">
         <v>122</v>
       </c>
-      <c r="C100" s="80"/>
-      <c r="D100" s="80"/>
-      <c r="E100" s="80"/>
-      <c r="F100" s="80"/>
-      <c r="G100" s="79"/>
-      <c r="H100" s="78" t="s">
+      <c r="C100" s="90"/>
+      <c r="D100" s="90"/>
+      <c r="E100" s="90"/>
+      <c r="F100" s="90"/>
+      <c r="G100" s="89"/>
+      <c r="H100" s="88" t="s">
         <v>123</v>
       </c>
-      <c r="I100" s="80"/>
-      <c r="J100" s="80"/>
-      <c r="K100" s="80"/>
-      <c r="L100" s="80"/>
-      <c r="M100" s="79"/>
+      <c r="I100" s="90"/>
+      <c r="J100" s="90"/>
+      <c r="K100" s="90"/>
+      <c r="L100" s="90"/>
+      <c r="M100" s="89"/>
     </row>
     <row r="101" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A101" s="87"/>
-      <c r="B101" s="78" t="s">
+      <c r="A101" s="82"/>
+      <c r="B101" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="C101" s="79"/>
-      <c r="D101" s="78" t="s">
+      <c r="C101" s="89"/>
+      <c r="D101" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="E101" s="79"/>
-      <c r="F101" s="78" t="s">
+      <c r="E101" s="89"/>
+      <c r="F101" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="G101" s="79"/>
-      <c r="H101" s="78" t="s">
+      <c r="G101" s="89"/>
+      <c r="H101" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="I101" s="79"/>
-      <c r="J101" s="78" t="s">
+      <c r="I101" s="89"/>
+      <c r="J101" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="K101" s="79"/>
-      <c r="L101" s="78" t="s">
+      <c r="K101" s="89"/>
+      <c r="L101" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="M101" s="79"/>
+      <c r="M101" s="89"/>
     </row>
     <row r="102" spans="1:13" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A102" s="87"/>
+      <c r="A102" s="82"/>
       <c r="B102" s="49" t="s">
         <v>10</v>
       </c>
@@ -5455,55 +5525,55 @@
       <c r="M115" s="57"/>
     </row>
     <row r="116" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A116" s="87" t="s">
+      <c r="A116" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="B116" s="78" t="s">
+      <c r="B116" s="88" t="s">
         <v>122</v>
       </c>
-      <c r="C116" s="80"/>
-      <c r="D116" s="80"/>
-      <c r="E116" s="80"/>
-      <c r="F116" s="80"/>
-      <c r="G116" s="79"/>
-      <c r="H116" s="78" t="s">
+      <c r="C116" s="90"/>
+      <c r="D116" s="90"/>
+      <c r="E116" s="90"/>
+      <c r="F116" s="90"/>
+      <c r="G116" s="89"/>
+      <c r="H116" s="88" t="s">
         <v>123</v>
       </c>
-      <c r="I116" s="80"/>
-      <c r="J116" s="80"/>
-      <c r="K116" s="80"/>
-      <c r="L116" s="80"/>
-      <c r="M116" s="79"/>
+      <c r="I116" s="90"/>
+      <c r="J116" s="90"/>
+      <c r="K116" s="90"/>
+      <c r="L116" s="90"/>
+      <c r="M116" s="89"/>
     </row>
     <row r="117" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A117" s="87"/>
-      <c r="B117" s="78" t="s">
+      <c r="A117" s="82"/>
+      <c r="B117" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="C117" s="79"/>
-      <c r="D117" s="78" t="s">
+      <c r="C117" s="89"/>
+      <c r="D117" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="E117" s="79"/>
-      <c r="F117" s="78" t="s">
+      <c r="E117" s="89"/>
+      <c r="F117" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="G117" s="79"/>
-      <c r="H117" s="78" t="s">
+      <c r="G117" s="89"/>
+      <c r="H117" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="I117" s="79"/>
-      <c r="J117" s="78" t="s">
+      <c r="I117" s="89"/>
+      <c r="J117" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="K117" s="79"/>
-      <c r="L117" s="78" t="s">
+      <c r="K117" s="89"/>
+      <c r="L117" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="M117" s="79"/>
+      <c r="M117" s="89"/>
     </row>
     <row r="118" spans="1:13" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A118" s="87"/>
+      <c r="A118" s="82"/>
       <c r="B118" s="49" t="s">
         <v>10</v>
       </c>
@@ -5993,57 +6063,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="64">
-    <mergeCell ref="P89:R89"/>
-    <mergeCell ref="P83:R83"/>
-    <mergeCell ref="P74:R74"/>
-    <mergeCell ref="P69:R69"/>
-    <mergeCell ref="O83:O85"/>
-    <mergeCell ref="R84:R85"/>
-    <mergeCell ref="O69:O71"/>
-    <mergeCell ref="R70:R71"/>
-    <mergeCell ref="H69:M69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="H70:I70"/>
-    <mergeCell ref="J70:K70"/>
-    <mergeCell ref="L70:M70"/>
-    <mergeCell ref="A69:A71"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="A100:A102"/>
-    <mergeCell ref="B100:G100"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="F101:G101"/>
-    <mergeCell ref="L86:M86"/>
-    <mergeCell ref="H117:I117"/>
-    <mergeCell ref="J117:K117"/>
-    <mergeCell ref="L117:M117"/>
-    <mergeCell ref="H85:M85"/>
-    <mergeCell ref="H116:M116"/>
-    <mergeCell ref="J86:K86"/>
-    <mergeCell ref="H100:M100"/>
-    <mergeCell ref="H101:I101"/>
-    <mergeCell ref="J101:K101"/>
-    <mergeCell ref="L101:M101"/>
-    <mergeCell ref="A116:A118"/>
-    <mergeCell ref="B116:G116"/>
-    <mergeCell ref="H86:I86"/>
-    <mergeCell ref="B117:C117"/>
-    <mergeCell ref="D117:E117"/>
-    <mergeCell ref="F117:G117"/>
-    <mergeCell ref="B86:C86"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="A85:A87"/>
-    <mergeCell ref="B85:G85"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
+  <mergeCells count="69">
+    <mergeCell ref="U87:V87"/>
+    <mergeCell ref="T69:T71"/>
+    <mergeCell ref="U69:V69"/>
+    <mergeCell ref="T83:T85"/>
+    <mergeCell ref="U83:V83"/>
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="H19:K19"/>
     <mergeCell ref="H36:K36"/>
@@ -6058,6 +6083,56 @@
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="H53:K53"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A116:A118"/>
+    <mergeCell ref="B116:G116"/>
+    <mergeCell ref="H86:I86"/>
+    <mergeCell ref="B117:C117"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="B86:C86"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="A85:A87"/>
+    <mergeCell ref="B85:G85"/>
+    <mergeCell ref="L86:M86"/>
+    <mergeCell ref="H117:I117"/>
+    <mergeCell ref="J117:K117"/>
+    <mergeCell ref="L117:M117"/>
+    <mergeCell ref="H85:M85"/>
+    <mergeCell ref="H116:M116"/>
+    <mergeCell ref="J86:K86"/>
+    <mergeCell ref="H100:M100"/>
+    <mergeCell ref="H101:I101"/>
+    <mergeCell ref="J101:K101"/>
+    <mergeCell ref="L101:M101"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="A100:A102"/>
+    <mergeCell ref="B100:G100"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="F101:G101"/>
+    <mergeCell ref="H69:M69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="F70:G70"/>
+    <mergeCell ref="H70:I70"/>
+    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="L70:M70"/>
+    <mergeCell ref="P89:R89"/>
+    <mergeCell ref="P83:R83"/>
+    <mergeCell ref="P74:R74"/>
+    <mergeCell ref="P69:R69"/>
+    <mergeCell ref="O83:O85"/>
+    <mergeCell ref="R84:R85"/>
+    <mergeCell ref="O69:O71"/>
+    <mergeCell ref="R70:R71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6093,27 +6168,27 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70" t="s">
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="70" t="s">
+      <c r="J1" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70" t="s">
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
@@ -6679,48 +6754,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="67" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="69"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="73"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74" t="s">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74" t="s">
+      <c r="E2" s="78"/>
+      <c r="F2" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="74"/>
+      <c r="G2" s="78"/>
       <c r="H2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="70" t="s">
+      <c r="I2" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70" t="s">
+      <c r="J2" s="74"/>
+      <c r="K2" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="70"/>
+      <c r="L2" s="74"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -7113,48 +7188,48 @@
       <c r="H16" s="9"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="71" t="s">
+      <c r="A17" s="75" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="72"/>
-      <c r="C17" s="72"/>
-      <c r="D17" s="72"/>
-      <c r="E17" s="72"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="72"/>
-      <c r="H17" s="73"/>
-      <c r="I17" s="67" t="s">
+      <c r="B17" s="76"/>
+      <c r="C17" s="76"/>
+      <c r="D17" s="76"/>
+      <c r="E17" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="77"/>
+      <c r="I17" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="68"/>
-      <c r="K17" s="68"/>
-      <c r="L17" s="69"/>
+      <c r="J17" s="72"/>
+      <c r="K17" s="72"/>
+      <c r="L17" s="73"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74" t="s">
+      <c r="C18" s="78"/>
+      <c r="D18" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74" t="s">
+      <c r="E18" s="78"/>
+      <c r="F18" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="74"/>
+      <c r="G18" s="78"/>
       <c r="H18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I18" s="70" t="s">
+      <c r="I18" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="J18" s="70"/>
-      <c r="K18" s="70" t="s">
+      <c r="J18" s="74"/>
+      <c r="K18" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="L18" s="70"/>
+      <c r="L18" s="74"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
@@ -7556,12 +7631,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="I17:L17"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
@@ -7570,6 +7639,12 @@
     <mergeCell ref="F18:G18"/>
     <mergeCell ref="A17:H17"/>
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="I17:L17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7590,38 +7665,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="79" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75" t="s">
+      <c r="C2" s="79"/>
+      <c r="D2" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75" t="s">
+      <c r="E2" s="79"/>
+      <c r="F2" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="76" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
+      <c r="I2" s="80"/>
+      <c r="J2" s="80"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="24"/>
@@ -7873,38 +7948,38 @@
       <c r="G17" s="25"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="75" t="s">
+      <c r="A18" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="31"/>
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="77"/>
-      <c r="D19" s="77" t="s">
+      <c r="C19" s="81"/>
+      <c r="D19" s="81" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="77"/>
-      <c r="F19" s="77" t="s">
+      <c r="E19" s="81"/>
+      <c r="F19" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="77"/>
-      <c r="H19" s="76" t="s">
+      <c r="G19" s="81"/>
+      <c r="H19" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="I19" s="76"/>
-      <c r="J19" s="76"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="80"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="24"/>
@@ -8197,73 +8272,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="67" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="69"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="73"/>
       <c r="M1" s="9"/>
-      <c r="N1" s="71" t="s">
+      <c r="N1" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="73"/>
+      <c r="O1" s="76"/>
+      <c r="P1" s="76"/>
+      <c r="Q1" s="76"/>
+      <c r="R1" s="76"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="77"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74" t="s">
+      <c r="C2" s="78"/>
+      <c r="D2" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74" t="s">
+      <c r="E2" s="78"/>
+      <c r="F2" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="74"/>
+      <c r="G2" s="78"/>
       <c r="H2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="70" t="s">
+      <c r="I2" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70" t="s">
+      <c r="J2" s="74"/>
+      <c r="K2" s="74" t="s">
         <v>46</v>
       </c>
-      <c r="L2" s="70"/>
+      <c r="L2" s="74"/>
       <c r="M2" s="9"/>
       <c r="N2" s="4"/>
-      <c r="O2" s="71" t="s">
+      <c r="O2" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="73"/>
-      <c r="Q2" s="71" t="s">
+      <c r="P2" s="77"/>
+      <c r="Q2" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="73"/>
-      <c r="S2" s="71" t="s">
+      <c r="R2" s="77"/>
+      <c r="S2" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="73"/>
+      <c r="T2" s="77"/>
       <c r="U2" s="4" t="s">
         <v>25</v>
       </c>
@@ -8897,46 +8972,46 @@
       <c r="U15" s="9"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A16" s="71" t="s">
+      <c r="A16" s="75" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="72"/>
-      <c r="C16" s="72"/>
-      <c r="D16" s="72"/>
-      <c r="E16" s="72"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="72"/>
-      <c r="H16" s="73"/>
+      <c r="B16" s="76"/>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="77"/>
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
-      <c r="N16" s="71" t="s">
+      <c r="N16" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="O16" s="72"/>
-      <c r="P16" s="72"/>
-      <c r="Q16" s="72"/>
-      <c r="R16" s="72"/>
-      <c r="S16" s="72"/>
-      <c r="T16" s="72"/>
-      <c r="U16" s="73"/>
+      <c r="O16" s="76"/>
+      <c r="P16" s="76"/>
+      <c r="Q16" s="76"/>
+      <c r="R16" s="76"/>
+      <c r="S16" s="76"/>
+      <c r="T16" s="76"/>
+      <c r="U16" s="77"/>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74" t="s">
+      <c r="C17" s="78"/>
+      <c r="D17" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74" t="s">
+      <c r="E17" s="78"/>
+      <c r="F17" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="74"/>
+      <c r="G17" s="78"/>
       <c r="H17" s="4" t="s">
         <v>25</v>
       </c>
@@ -8946,18 +9021,18 @@
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
       <c r="N17" s="4"/>
-      <c r="O17" s="71" t="s">
+      <c r="O17" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="P17" s="73"/>
-      <c r="Q17" s="71" t="s">
+      <c r="P17" s="77"/>
+      <c r="Q17" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="R17" s="73"/>
-      <c r="S17" s="71" t="s">
+      <c r="R17" s="77"/>
+      <c r="S17" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="T17" s="73"/>
+      <c r="T17" s="77"/>
       <c r="U17" s="4" t="s">
         <v>25</v>
       </c>
@@ -9510,6 +9585,12 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="N1:U1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="O2:P2"/>
     <mergeCell ref="Q17:R17"/>
     <mergeCell ref="S17:T17"/>
     <mergeCell ref="N16:U16"/>
@@ -9523,12 +9604,6 @@
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="F17:G17"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="N1:U1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="O2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9551,79 +9626,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
+      <c r="B1" s="78"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
       <c r="L1" s="9"/>
       <c r="M1" s="27"/>
-      <c r="N1" s="74" t="s">
+      <c r="N1" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="74"/>
-      <c r="P1" s="74"/>
-      <c r="Q1" s="74"/>
-      <c r="R1" s="74"/>
-      <c r="S1" s="74"/>
-      <c r="T1" s="74"/>
-      <c r="U1" s="74"/>
-      <c r="V1" s="74"/>
+      <c r="O1" s="78"/>
+      <c r="P1" s="78"/>
+      <c r="Q1" s="78"/>
+      <c r="R1" s="78"/>
+      <c r="S1" s="78"/>
+      <c r="T1" s="78"/>
+      <c r="U1" s="78"/>
+      <c r="V1" s="78"/>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75" t="s">
+      <c r="C2" s="79"/>
+      <c r="D2" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75" t="s">
+      <c r="E2" s="79"/>
+      <c r="F2" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75" t="s">
+      <c r="G2" s="79"/>
+      <c r="H2" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="75"/>
-      <c r="J2" s="76" t="s">
+      <c r="I2" s="79"/>
+      <c r="J2" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
+      <c r="K2" s="80"/>
+      <c r="L2" s="80"/>
       <c r="M2" s="25"/>
       <c r="N2" s="24"/>
-      <c r="O2" s="75" t="s">
+      <c r="O2" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="P2" s="75"/>
-      <c r="Q2" s="75" t="s">
+      <c r="P2" s="79"/>
+      <c r="Q2" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="75"/>
-      <c r="S2" s="75" t="s">
+      <c r="R2" s="79"/>
+      <c r="S2" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75" t="s">
+      <c r="T2" s="79"/>
+      <c r="U2" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="75"/>
-      <c r="W2" s="76" t="s">
+      <c r="V2" s="79"/>
+      <c r="W2" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="X2" s="76"/>
-      <c r="Y2" s="76"/>
+      <c r="X2" s="80"/>
+      <c r="Y2" s="80"/>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="24"/>
@@ -10334,82 +10409,82 @@
       <c r="Y17" s="25"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A18" s="75" t="s">
+      <c r="A18" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
+      <c r="B18" s="79"/>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
       <c r="J18" s="25"/>
       <c r="K18" s="25"/>
       <c r="L18" s="25"/>
       <c r="M18" s="25"/>
-      <c r="N18" s="75" t="s">
+      <c r="N18" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="O18" s="75"/>
-      <c r="P18" s="75"/>
-      <c r="Q18" s="75"/>
-      <c r="R18" s="75"/>
-      <c r="S18" s="75"/>
-      <c r="T18" s="75"/>
-      <c r="U18" s="75"/>
-      <c r="V18" s="75"/>
+      <c r="O18" s="79"/>
+      <c r="P18" s="79"/>
+      <c r="Q18" s="79"/>
+      <c r="R18" s="79"/>
+      <c r="S18" s="79"/>
+      <c r="T18" s="79"/>
+      <c r="U18" s="79"/>
+      <c r="V18" s="79"/>
       <c r="W18" s="25"/>
       <c r="X18" s="25"/>
       <c r="Y18" s="25"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="24"/>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="75"/>
-      <c r="D19" s="75" t="s">
+      <c r="C19" s="79"/>
+      <c r="D19" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75" t="s">
+      <c r="E19" s="79"/>
+      <c r="F19" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75" t="s">
+      <c r="G19" s="79"/>
+      <c r="H19" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="I19" s="75"/>
-      <c r="J19" s="76" t="s">
+      <c r="I19" s="79"/>
+      <c r="J19" s="80" t="s">
         <v>79</v>
       </c>
-      <c r="K19" s="76"/>
-      <c r="L19" s="76"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="80"/>
       <c r="M19" s="25"/>
       <c r="N19" s="24"/>
-      <c r="O19" s="75" t="s">
+      <c r="O19" s="79" t="s">
         <v>0</v>
       </c>
-      <c r="P19" s="75"/>
-      <c r="Q19" s="75" t="s">
+      <c r="P19" s="79"/>
+      <c r="Q19" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="R19" s="75"/>
-      <c r="S19" s="75" t="s">
+      <c r="R19" s="79"/>
+      <c r="S19" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="T19" s="75"/>
-      <c r="U19" s="75" t="s">
+      <c r="T19" s="79"/>
+      <c r="U19" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="V19" s="75"/>
-      <c r="W19" s="75" t="s">
+      <c r="V19" s="79"/>
+      <c r="W19" s="79" t="s">
         <v>79</v>
       </c>
-      <c r="X19" s="75"/>
-      <c r="Y19" s="75"/>
+      <c r="X19" s="79"/>
+      <c r="Y19" s="79"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="24"/>
@@ -10947,6 +11022,15 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="W19:Y19"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="W2:Y2"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="U19:V19"/>
     <mergeCell ref="U2:V2"/>
@@ -10962,15 +11046,6 @@
     <mergeCell ref="Q19:R19"/>
     <mergeCell ref="S19:T19"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="W19:Y19"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="W2:Y2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15274,10 +15349,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E87A03-7511-4C2E-B4E0-ED136DA0DD22}">
-  <dimension ref="A1:S67"/>
+  <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P54" sqref="P54:Q54"/>
+    <sheetView tabSelected="1" topLeftCell="C51" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q71" sqref="Q71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15289,36 +15364,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" s="81" t="s">
+      <c r="A1" s="92" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="83"/>
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="94"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="24"/>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="C2" s="83"/>
-      <c r="D2" s="81" t="s">
+      <c r="C2" s="94"/>
+      <c r="D2" s="92" t="s">
         <v>117</v>
       </c>
-      <c r="E2" s="83"/>
-      <c r="F2" s="81" t="s">
+      <c r="E2" s="94"/>
+      <c r="F2" s="92" t="s">
         <v>118</v>
       </c>
-      <c r="G2" s="83"/>
-      <c r="H2" s="67" t="s">
+      <c r="G2" s="94"/>
+      <c r="H2" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="68"/>
-      <c r="J2" s="68"/>
-      <c r="K2" s="69"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="73"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
@@ -15466,17 +15541,17 @@
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-      <c r="O7" s="95" t="s">
+      <c r="O7" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="P7" s="96" t="s">
+      <c r="P7" s="88" t="s">
         <v>133</v>
       </c>
-      <c r="Q7" s="97"/>
-      <c r="R7" s="96" t="s">
+      <c r="Q7" s="89"/>
+      <c r="R7" s="88" t="s">
         <v>134</v>
       </c>
-      <c r="S7" s="97"/>
+      <c r="S7" s="89"/>
     </row>
     <row r="8" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -15504,17 +15579,17 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="O8" s="95"/>
-      <c r="P8" s="98" t="s">
+      <c r="O8" s="82"/>
+      <c r="P8" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="Q8" s="98" t="s">
+      <c r="Q8" s="67" t="s">
         <v>136</v>
       </c>
-      <c r="R8" s="98" t="s">
+      <c r="R8" s="67" t="s">
         <v>135</v>
       </c>
-      <c r="S8" s="98" t="s">
+      <c r="S8" s="67" t="s">
         <v>136</v>
       </c>
     </row>
@@ -15544,17 +15619,17 @@
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-      <c r="O9" s="95"/>
-      <c r="P9" s="99" t="s">
+      <c r="O9" s="82"/>
+      <c r="P9" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="Q9" s="99" t="s">
+      <c r="Q9" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="R9" s="99" t="s">
+      <c r="R9" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="S9" s="99" t="s">
+      <c r="S9" s="49" t="s">
         <v>137</v>
       </c>
     </row>
@@ -15584,19 +15659,19 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="O10" s="100" t="s">
+      <c r="O10" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="P10" s="101" t="s">
+      <c r="P10" s="53" t="s">
         <v>176</v>
       </c>
-      <c r="Q10" s="101" t="s">
+      <c r="Q10" s="53" t="s">
         <v>178</v>
       </c>
-      <c r="R10" s="101" t="s">
+      <c r="R10" s="53" t="s">
         <v>175</v>
       </c>
-      <c r="S10" s="101" t="s">
+      <c r="S10" s="53" t="s">
         <v>177</v>
       </c>
     </row>
@@ -15630,19 +15705,19 @@
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-      <c r="O11" s="100" t="s">
+      <c r="O11" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P11" s="99" t="s">
+      <c r="P11" s="49" t="s">
         <v>183</v>
       </c>
-      <c r="Q11" s="99" t="s">
+      <c r="Q11" s="49" t="s">
         <v>185</v>
       </c>
-      <c r="R11" s="99" t="s">
+      <c r="R11" s="49" t="s">
         <v>222</v>
       </c>
-      <c r="S11" s="99" t="s">
+      <c r="S11" s="49" t="s">
         <v>184</v>
       </c>
     </row>
@@ -15672,19 +15747,19 @@
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="O12" s="100" t="s">
+      <c r="O12" s="54" t="s">
         <v>104</v>
       </c>
-      <c r="P12" s="99" t="s">
+      <c r="P12" s="49" t="s">
         <v>187</v>
       </c>
-      <c r="Q12" s="99" t="s">
+      <c r="Q12" s="49" t="s">
         <v>189</v>
       </c>
-      <c r="R12" s="99" t="s">
+      <c r="R12" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="S12" s="99" t="s">
+      <c r="S12" s="49" t="s">
         <v>188</v>
       </c>
     </row>
@@ -15714,19 +15789,19 @@
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-      <c r="O13" s="100" t="s">
+      <c r="O13" s="54" t="s">
         <v>105</v>
       </c>
-      <c r="P13" s="99" t="s">
+      <c r="P13" s="49" t="s">
         <v>191</v>
       </c>
-      <c r="Q13" s="99" t="s">
+      <c r="Q13" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="R13" s="99" t="s">
+      <c r="R13" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="S13" s="99" t="s">
+      <c r="S13" s="49" t="s">
         <v>192</v>
       </c>
     </row>
@@ -15756,24 +15831,24 @@
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="O14" s="100" t="s">
+      <c r="O14" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="P14" s="99" t="s">
+      <c r="P14" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="Q14" s="99" t="s">
+      <c r="Q14" s="49" t="s">
         <v>197</v>
       </c>
-      <c r="R14" s="99" t="s">
+      <c r="R14" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="S14" s="99" t="s">
+      <c r="S14" s="49" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="91" t="s">
+      <c r="A15" s="68" t="s">
         <v>113</v>
       </c>
       <c r="B15" s="24">
@@ -15798,19 +15873,19 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
-      <c r="O15" s="100" t="s">
+      <c r="O15" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="P15" s="99" t="s">
+      <c r="P15" s="49" t="s">
         <v>199</v>
       </c>
-      <c r="Q15" s="99" t="s">
+      <c r="Q15" s="49" t="s">
         <v>201</v>
       </c>
-      <c r="R15" s="99" t="s">
+      <c r="R15" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="S15" s="99" t="s">
+      <c r="S15" s="49" t="s">
         <v>200</v>
       </c>
     </row>
@@ -15822,19 +15897,19 @@
       <c r="E16" s="25"/>
       <c r="F16" s="25"/>
       <c r="G16" s="25"/>
-      <c r="O16" s="100" t="s">
+      <c r="O16" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="P16" s="99" t="s">
+      <c r="P16" s="49" t="s">
         <v>203</v>
       </c>
-      <c r="Q16" s="99" t="s">
+      <c r="Q16" s="49" t="s">
         <v>205</v>
       </c>
-      <c r="R16" s="99" t="s">
+      <c r="R16" s="49" t="s">
         <v>202</v>
       </c>
-      <c r="S16" s="99" t="s">
+      <c r="S16" s="49" t="s">
         <v>204</v>
       </c>
     </row>
@@ -15846,81 +15921,81 @@
       <c r="E17" s="25"/>
       <c r="F17" s="25"/>
       <c r="G17" s="25"/>
-      <c r="O17" s="100" t="s">
+      <c r="O17" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="P17" s="101" t="s">
+      <c r="P17" s="53" t="s">
         <v>180</v>
       </c>
-      <c r="Q17" s="101" t="s">
+      <c r="Q17" s="53" t="s">
         <v>182</v>
       </c>
-      <c r="R17" s="99" t="s">
+      <c r="R17" s="49" t="s">
         <v>179</v>
       </c>
-      <c r="S17" s="99" t="s">
+      <c r="S17" s="49" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="81" t="s">
+      <c r="A18" s="92" t="s">
         <v>115</v>
       </c>
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="82"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="82"/>
-      <c r="G18" s="83"/>
-      <c r="O18" s="100" t="s">
+      <c r="B18" s="93"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="93"/>
+      <c r="F18" s="93"/>
+      <c r="G18" s="94"/>
+      <c r="O18" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="P18" s="99" t="s">
+      <c r="P18" s="49" t="s">
         <v>210</v>
       </c>
-      <c r="Q18" s="99" t="s">
+      <c r="Q18" s="49" t="s">
         <v>212</v>
       </c>
-      <c r="R18" s="99" t="s">
+      <c r="R18" s="49" t="s">
         <v>211</v>
       </c>
-      <c r="S18" s="99" t="s">
+      <c r="S18" s="49" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="31"/>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="92" t="s">
         <v>116</v>
       </c>
-      <c r="C19" s="83"/>
-      <c r="D19" s="81" t="s">
+      <c r="C19" s="94"/>
+      <c r="D19" s="92" t="s">
         <v>120</v>
       </c>
-      <c r="E19" s="83"/>
-      <c r="F19" s="81" t="s">
+      <c r="E19" s="94"/>
+      <c r="F19" s="92" t="s">
         <v>118</v>
       </c>
-      <c r="G19" s="83"/>
-      <c r="H19" s="67" t="s">
+      <c r="G19" s="94"/>
+      <c r="H19" s="71" t="s">
         <v>119</v>
       </c>
-      <c r="I19" s="68"/>
-      <c r="J19" s="68"/>
-      <c r="K19" s="69"/>
-      <c r="O19" s="100" t="s">
+      <c r="I19" s="72"/>
+      <c r="J19" s="72"/>
+      <c r="K19" s="73"/>
+      <c r="O19" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="P19" s="99" t="s">
+      <c r="P19" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="Q19" s="99" t="s">
+      <c r="Q19" s="49" t="s">
         <v>216</v>
       </c>
-      <c r="R19" s="99" t="s">
+      <c r="R19" s="49" t="s">
         <v>215</v>
       </c>
-      <c r="S19" s="99" t="s">
+      <c r="S19" s="49" t="s">
         <v>217</v>
       </c>
     </row>
@@ -15958,19 +16033,19 @@
       <c r="K20" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="O20" s="100" t="s">
+      <c r="O20" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="P20" s="99" t="s">
+      <c r="P20" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="Q20" s="99" t="s">
+      <c r="Q20" s="49" t="s">
         <v>221</v>
       </c>
-      <c r="R20" s="99" t="s">
+      <c r="R20" s="49" t="s">
         <v>218</v>
       </c>
-      <c r="S20" s="99" t="s">
+      <c r="S20" s="49" t="s">
         <v>220</v>
       </c>
     </row>
@@ -16004,19 +16079,19 @@
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-      <c r="O21" s="102" t="s">
+      <c r="O21" s="55" t="s">
         <v>113</v>
       </c>
-      <c r="P21" s="99" t="s">
+      <c r="P21" s="49" t="s">
         <v>207</v>
       </c>
-      <c r="Q21" s="99" t="s">
+      <c r="Q21" s="49" t="s">
         <v>209</v>
       </c>
-      <c r="R21" s="99" t="s">
+      <c r="R21" s="49" t="s">
         <v>206</v>
       </c>
-      <c r="S21" s="99" t="s">
+      <c r="S21" s="49" t="s">
         <v>208</v>
       </c>
     </row>
@@ -16303,7 +16378,7 @@
       <c r="K31" s="4"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A32" s="91" t="s">
+      <c r="A32" s="68" t="s">
         <v>113</v>
       </c>
       <c r="B32" s="24">
@@ -16330,55 +16405,55 @@
       <c r="K32" s="1"/>
     </row>
     <row r="35" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="84" t="s">
+      <c r="A35" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="B35" s="78" t="s">
+      <c r="B35" s="88" t="s">
         <v>128</v>
       </c>
-      <c r="C35" s="80"/>
-      <c r="D35" s="80"/>
-      <c r="E35" s="80"/>
-      <c r="F35" s="80"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="78" t="s">
+      <c r="C35" s="90"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="89"/>
+      <c r="H35" s="88" t="s">
         <v>129</v>
       </c>
-      <c r="I35" s="80"/>
-      <c r="J35" s="80"/>
-      <c r="K35" s="80"/>
-      <c r="L35" s="80"/>
-      <c r="M35" s="79"/>
+      <c r="I35" s="90"/>
+      <c r="J35" s="90"/>
+      <c r="K35" s="90"/>
+      <c r="L35" s="90"/>
+      <c r="M35" s="89"/>
     </row>
     <row r="36" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="85"/>
-      <c r="B36" s="78" t="s">
+      <c r="A36" s="91"/>
+      <c r="B36" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="C36" s="79"/>
-      <c r="D36" s="78" t="s">
+      <c r="C36" s="89"/>
+      <c r="D36" s="88" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="79"/>
-      <c r="F36" s="78" t="s">
+      <c r="E36" s="89"/>
+      <c r="F36" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="G36" s="79"/>
-      <c r="H36" s="78" t="s">
+      <c r="G36" s="89"/>
+      <c r="H36" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="I36" s="79"/>
-      <c r="J36" s="78" t="s">
+      <c r="I36" s="89"/>
+      <c r="J36" s="88" t="s">
         <v>120</v>
       </c>
-      <c r="K36" s="79"/>
-      <c r="L36" s="78" t="s">
+      <c r="K36" s="89"/>
+      <c r="L36" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="M36" s="79"/>
+      <c r="M36" s="89"/>
     </row>
     <row r="37" spans="1:13" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A37" s="86"/>
+      <c r="A37" s="84"/>
       <c r="B37" s="49" t="s">
         <v>10</v>
       </c>
@@ -16868,7 +16943,7 @@
       </c>
     </row>
     <row r="49" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A49" s="103" t="s">
+      <c r="A49" s="69" t="s">
         <v>113</v>
       </c>
       <c r="B49" s="49">
@@ -16909,17 +16984,17 @@
       </c>
     </row>
     <row r="50" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A50" s="92"/>
-      <c r="B50" s="93"/>
-      <c r="C50" s="93"/>
-      <c r="D50" s="93"/>
-      <c r="E50" s="93"/>
-      <c r="G50" s="93"/>
-      <c r="H50" s="93"/>
-      <c r="I50" s="93"/>
-      <c r="J50" s="93"/>
-      <c r="K50" s="93"/>
-      <c r="M50" s="94"/>
+      <c r="A50" s="57"/>
+      <c r="B50" s="56"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="G50" s="56"/>
+      <c r="H50" s="56"/>
+      <c r="I50" s="56"/>
+      <c r="J50" s="56"/>
+      <c r="K50" s="56"/>
+      <c r="M50" s="47"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A51" s="25"/>
@@ -16940,73 +17015,73 @@
       <c r="G52" s="25"/>
     </row>
     <row r="53" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A53" s="84" t="s">
+      <c r="A53" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="B53" s="78" t="s">
+      <c r="B53" s="88" t="s">
         <v>128</v>
       </c>
-      <c r="C53" s="80"/>
-      <c r="D53" s="80"/>
-      <c r="E53" s="80"/>
-      <c r="F53" s="80"/>
-      <c r="G53" s="79"/>
-      <c r="H53" s="78" t="s">
+      <c r="C53" s="90"/>
+      <c r="D53" s="90"/>
+      <c r="E53" s="90"/>
+      <c r="F53" s="90"/>
+      <c r="G53" s="89"/>
+      <c r="H53" s="88" t="s">
         <v>129</v>
       </c>
-      <c r="I53" s="80"/>
-      <c r="J53" s="80"/>
-      <c r="K53" s="80"/>
-      <c r="L53" s="80"/>
-      <c r="M53" s="79"/>
-      <c r="O53" s="87" t="s">
+      <c r="I53" s="90"/>
+      <c r="J53" s="90"/>
+      <c r="K53" s="90"/>
+      <c r="L53" s="90"/>
+      <c r="M53" s="89"/>
+      <c r="O53" s="82" t="s">
         <v>116</v>
       </c>
-      <c r="P53" s="105" t="s">
+      <c r="P53" s="85" t="s">
         <v>139</v>
       </c>
-      <c r="Q53" s="106"/>
-      <c r="R53" s="107"/>
+      <c r="Q53" s="86"/>
+      <c r="R53" s="87"/>
     </row>
     <row r="54" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A54" s="85"/>
-      <c r="B54" s="78" t="s">
+      <c r="A54" s="91"/>
+      <c r="B54" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="C54" s="79"/>
-      <c r="D54" s="78" t="s">
+      <c r="C54" s="89"/>
+      <c r="D54" s="88" t="s">
         <v>117</v>
       </c>
-      <c r="E54" s="79"/>
-      <c r="F54" s="78" t="s">
+      <c r="E54" s="89"/>
+      <c r="F54" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="G54" s="79"/>
-      <c r="H54" s="78" t="s">
+      <c r="G54" s="89"/>
+      <c r="H54" s="88" t="s">
         <v>116</v>
       </c>
-      <c r="I54" s="79"/>
-      <c r="J54" s="78" t="s">
+      <c r="I54" s="89"/>
+      <c r="J54" s="88" t="s">
         <v>120</v>
       </c>
-      <c r="K54" s="79"/>
-      <c r="L54" s="78" t="s">
+      <c r="K54" s="89"/>
+      <c r="L54" s="88" t="s">
         <v>118</v>
       </c>
-      <c r="M54" s="79"/>
-      <c r="O54" s="87"/>
+      <c r="M54" s="89"/>
+      <c r="O54" s="82"/>
       <c r="P54" s="49" t="s">
         <v>223</v>
       </c>
       <c r="Q54" s="49" t="s">
         <v>224</v>
       </c>
-      <c r="R54" s="84" t="s">
+      <c r="R54" s="83" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.3">
-      <c r="A55" s="86"/>
+      <c r="A55" s="84"/>
       <c r="B55" s="49" t="s">
         <v>10</v>
       </c>
@@ -17043,14 +17118,14 @@
       <c r="M55" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="O55" s="87"/>
+      <c r="O55" s="82"/>
       <c r="P55" s="49" t="s">
         <v>137</v>
       </c>
       <c r="Q55" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="R55" s="86"/>
+      <c r="R55" s="84"/>
       <c r="S55" s="64"/>
     </row>
     <row r="56" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
@@ -17200,12 +17275,12 @@
       <c r="M58" s="48">
         <v>0.04</v>
       </c>
-      <c r="O58" s="104"/>
-      <c r="P58" s="105" t="s">
+      <c r="O58" s="70"/>
+      <c r="P58" s="85" t="s">
         <v>140</v>
       </c>
-      <c r="Q58" s="106"/>
-      <c r="R58" s="107"/>
+      <c r="Q58" s="86"/>
+      <c r="R58" s="87"/>
     </row>
     <row r="59" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="54" t="s">
@@ -17501,7 +17576,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="54" t="s">
         <v>109</v>
       </c>
@@ -17541,8 +17616,15 @@
       <c r="M65" s="52">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="66" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O65" s="82" t="s">
+        <v>116</v>
+      </c>
+      <c r="P65" s="82" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q65" s="82"/>
+    </row>
+    <row r="66" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="54" t="s">
         <v>110</v>
       </c>
@@ -17582,9 +17664,16 @@
       <c r="M66" s="52">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="67" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A67" s="103" t="s">
+      <c r="O66" s="82"/>
+      <c r="P66" s="49" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q66" s="49" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="69" t="s">
         <v>113</v>
       </c>
       <c r="B67" s="49">
@@ -17623,28 +17712,29 @@
       <c r="M67" s="49">
         <v>0.09</v>
       </c>
+      <c r="O67" s="82"/>
+      <c r="P67" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q67" s="49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="O68" s="54" t="s">
+        <v>138</v>
+      </c>
+      <c r="P68" s="65">
+        <v>0.01</v>
+      </c>
+      <c r="Q68" s="65">
+        <v>0.15</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="O53:O55"/>
-    <mergeCell ref="R54:R55"/>
-    <mergeCell ref="P58:R58"/>
-    <mergeCell ref="P53:R53"/>
-    <mergeCell ref="O7:O9"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="R7:S7"/>
-    <mergeCell ref="H53:M53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="L54:M54"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B35:G35"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:G53"/>
+  <mergeCells count="37">
+    <mergeCell ref="O65:O67"/>
+    <mergeCell ref="P65:Q65"/>
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="J36:K36"/>
     <mergeCell ref="L36:M36"/>
@@ -17661,6 +17751,25 @@
     <mergeCell ref="H19:K19"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B35:G35"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:G53"/>
+    <mergeCell ref="H53:M53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="H54:I54"/>
+    <mergeCell ref="J54:K54"/>
+    <mergeCell ref="L54:M54"/>
+    <mergeCell ref="O53:O55"/>
+    <mergeCell ref="R54:R55"/>
+    <mergeCell ref="P58:R58"/>
+    <mergeCell ref="P53:R53"/>
+    <mergeCell ref="O7:O9"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="R7:S7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>